<commit_message>
parameter editting scripts added; some tests modified the xlsx files
</commit_message>
<xml_diff>
--- a/onset_detection/VR_Tendon_chan_2_para.xlsx
+++ b/onset_detection/VR_Tendon_chan_2_para.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -230,6 +230,74 @@
   <si>
     <t>Group data proc: 
 min_onset_allowed (N_sample)</t>
+  </si>
+  <si>
+    <t>Group data proc: 
+qViewTrialByTrial</t>
+  </si>
+  <si>
+    <t>RangeInputBox</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>iTrial</t>
+  </si>
+  <si>
+    <t>iChannel</t>
+  </si>
+  <si>
+    <t>should be the same cross-channel:
+min_Length</t>
+  </si>
+  <si>
+    <t>high_threshold</t>
+  </si>
+  <si>
+    <t>min_duration</t>
+  </si>
+  <si>
+    <t>min_n_sample</t>
+  </si>
+  <si>
+    <t>peak_direction</t>
+  </si>
+  <si>
+    <t>iSolution</t>
+  </si>
+  <si>
+    <t>wtc_frequency</t>
+  </si>
+  <si>
+    <t>wtc_signma_thres</t>
+  </si>
+  <si>
+    <t>qPlot</t>
+  </si>
+  <si>
+    <t>Group data proc:
+ nStartTrial</t>
+  </si>
+  <si>
+    <t>Group data proc: 
+nEndTrial</t>
+  </si>
+  <si>
+    <t>Group data proc: 
+min_onset_allowed (N_sample)</t>
+  </si>
+  <si>
+    <t>Group data proc: 
+max_onset_allowed (N_sample)</t>
+  </si>
+  <si>
+    <t>Group data proc: 
+min_diff_allowed (second)</t>
+  </si>
+  <si>
+    <t>Group data proc: 
+max_diff_allowed (second)</t>
   </si>
   <si>
     <t>Group data proc: 
@@ -257,7 +325,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -269,16 +337,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,7 +358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="true"/>
@@ -304,13 +374,13 @@
         <v>200</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E1" s="0">
         <v>1</v>
@@ -324,13 +394,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E2" s="0">
         <v>1</v>
@@ -344,13 +414,13 @@
         <v>1000</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E3" s="0">
         <v>1</v>
@@ -364,13 +434,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E4" s="0">
         <v>-10</v>
@@ -384,13 +454,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E5" s="0">
         <v>1</v>
@@ -404,13 +474,13 @@
         <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E6" s="0">
         <v>1</v>
@@ -424,13 +494,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E7" s="0">
         <v>-1</v>
@@ -444,13 +514,13 @@
         <v>135</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E8" s="0">
         <v>0</v>
@@ -464,13 +534,13 @@
         <v>37</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E9" s="0">
         <v>1</v>
@@ -484,13 +554,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E10" s="0">
         <v>0</v>
@@ -504,13 +574,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E11" s="0">
         <v>0</v>
@@ -524,13 +594,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E12" s="0">
         <v>1</v>
@@ -544,13 +614,13 @@
         <v>350</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E13" s="0">
         <v>1</v>
@@ -564,13 +634,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E14" s="0">
         <v>0</v>
@@ -581,21 +651,81 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E15" s="0">
         <v>0</v>
       </c>
       <c r="F15" s="0">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>1</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="0">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>1</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="0">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>0</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="0">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>